<commit_message>
Aryan bro's Web Labs which didnt help
</commit_message>
<xml_diff>
--- a/ToA/Mids Marks List.xlsx
+++ b/ToA/Mids Marks List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wali\Documents\Projects\6thSemester\ToA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04872B3F-D3E8-4CCA-AEB4-92218F84839C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E8B91B-4B04-4F18-AA66-927309270A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1176,7 +1176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1268,6 +1268,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1292,23 +1298,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1316,16 +1319,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1621,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1646,10 +1639,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="40" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="32" t="s">
@@ -1660,7 +1653,7 @@
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
       <c r="H1" s="32"/>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="35" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="32" t="s">
@@ -1673,7 +1666,7 @@
       </c>
       <c r="N1" s="32"/>
       <c r="O1" s="32"/>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="33" t="s">
         <v>9</v>
       </c>
       <c r="Q1" s="32" t="s">
@@ -1688,7 +1681,7 @@
       <c r="X1" s="12"/>
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
-      <c r="AA1" s="41" t="s">
+      <c r="AA1" s="33" t="s">
         <v>9</v>
       </c>
       <c r="AB1" s="10" t="s">
@@ -1699,13 +1692,13 @@
       <c r="AE1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="AF1" s="42" t="s">
+      <c r="AF1" s="34" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" s="36"/>
-      <c r="B2" s="39"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1724,7 +1717,7 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="34"/>
+      <c r="I2" s="36"/>
       <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1743,7 +1736,7 @@
       <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="41"/>
+      <c r="P2" s="33"/>
       <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1768,7 +1761,7 @@
       <c r="X2" s="12"/>
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
-      <c r="AA2" s="41"/>
+      <c r="AA2" s="33"/>
       <c r="AB2" s="10" t="s">
         <v>3</v>
       </c>
@@ -1779,11 +1772,11 @@
         <v>5</v>
       </c>
       <c r="AE2" s="32"/>
-      <c r="AF2" s="42"/>
+      <c r="AF2" s="34"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
-      <c r="B3" s="39"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1857,11 +1850,11 @@
       <c r="AE3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AF3" s="42"/>
+      <c r="AF3" s="34"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="1">
         <v>6</v>
       </c>
@@ -1979,7 +1972,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="6">
-        <f>SUM(C5:H5)</f>
+        <f t="shared" ref="I5:I48" si="0">SUM(C5:H5)</f>
         <v>6</v>
       </c>
       <c r="J5" s="4"/>
@@ -2032,7 +2025,7 @@
         <v>4</v>
       </c>
       <c r="I6" s="6">
-        <f>SUM(C6:H6)</f>
+        <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
       <c r="J6" s="4"/>
@@ -2085,7 +2078,7 @@
         <v>4</v>
       </c>
       <c r="I7" s="6">
-        <f>SUM(C7:H7)</f>
+        <f t="shared" si="0"/>
         <v>26.5</v>
       </c>
       <c r="J7" s="4"/>
@@ -2138,7 +2131,7 @@
         <v>4</v>
       </c>
       <c r="I8" s="6">
-        <f>SUM(C8:H8)</f>
+        <f t="shared" si="0"/>
         <v>24.5</v>
       </c>
       <c r="J8" s="4"/>
@@ -2191,7 +2184,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="6">
-        <f>SUM(C9:H9)</f>
+        <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
       <c r="J9" s="4"/>
@@ -2244,7 +2237,7 @@
         <v>4</v>
       </c>
       <c r="I10" s="6">
-        <f>SUM(C10:H10)</f>
+        <f t="shared" si="0"/>
         <v>19.5</v>
       </c>
       <c r="J10" s="4"/>
@@ -2297,7 +2290,7 @@
         <v>4</v>
       </c>
       <c r="I11" s="6">
-        <f>SUM(C11:H11)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="J11" s="4"/>
@@ -2350,7 +2343,7 @@
         <v>3</v>
       </c>
       <c r="I12" s="6">
-        <f>SUM(C12:H12)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="J12" s="4"/>
@@ -2403,7 +2396,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="6">
-        <f>SUM(C13:H13)</f>
+        <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
       <c r="J13" s="4"/>
@@ -2456,7 +2449,7 @@
         <v>4</v>
       </c>
       <c r="I14" s="6">
-        <f>SUM(C14:H14)</f>
+        <f t="shared" si="0"/>
         <v>20.5</v>
       </c>
       <c r="J14" s="4"/>
@@ -2509,7 +2502,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="6">
-        <f>SUM(C15:H15)</f>
+        <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
       <c r="J15" s="4"/>
@@ -2562,7 +2555,7 @@
         <v>4</v>
       </c>
       <c r="I16" s="6">
-        <f>SUM(C16:H16)</f>
+        <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
       <c r="J16" s="4"/>
@@ -2615,7 +2608,7 @@
         <v>4</v>
       </c>
       <c r="I17" s="6">
-        <f>SUM(C17:H17)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="J17" s="4"/>
@@ -2668,7 +2661,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="6">
-        <f>SUM(C18:H18)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="J18" s="4"/>
@@ -2721,7 +2714,7 @@
         <v>4</v>
       </c>
       <c r="I19" s="6">
-        <f>SUM(C19:H19)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="J19" s="4"/>
@@ -2774,7 +2767,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="6">
-        <f>SUM(C20:H20)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="J20" s="4"/>
@@ -2827,7 +2820,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="6">
-        <f>SUM(C21:H21)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="J21" s="4"/>
@@ -2880,7 +2873,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="6">
-        <f>SUM(C22:H22)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="J22" s="4"/>
@@ -2933,7 +2926,7 @@
         <v>4</v>
       </c>
       <c r="I23" s="6">
-        <f>SUM(C23:H23)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="J23" s="4"/>
@@ -2986,7 +2979,7 @@
         <v>2</v>
       </c>
       <c r="I24" s="6">
-        <f>SUM(C24:H24)</f>
+        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="J24" s="4"/>
@@ -3039,7 +3032,7 @@
         <v>4</v>
       </c>
       <c r="I25" s="6">
-        <f>SUM(C25:H25)</f>
+        <f t="shared" si="0"/>
         <v>21.5</v>
       </c>
       <c r="J25" s="4"/>
@@ -3092,7 +3085,7 @@
         <v>3</v>
       </c>
       <c r="I26" s="6">
-        <f>SUM(C26:H26)</f>
+        <f t="shared" si="0"/>
         <v>19.5</v>
       </c>
       <c r="J26" s="4"/>
@@ -3145,7 +3138,7 @@
         <v>4</v>
       </c>
       <c r="I27" s="6">
-        <f>SUM(C27:H27)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="J27" s="4"/>
@@ -3198,7 +3191,7 @@
         <v>4</v>
       </c>
       <c r="I28" s="6">
-        <f>SUM(C28:H28)</f>
+        <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
       <c r="J28" s="4"/>
@@ -3251,7 +3244,7 @@
         <v>4</v>
       </c>
       <c r="I29" s="6">
-        <f>SUM(C29:H29)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="J29" s="4"/>
@@ -3304,7 +3297,7 @@
         <v>4</v>
       </c>
       <c r="I30" s="6">
-        <f>SUM(C30:H30)</f>
+        <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
       <c r="J30" s="4"/>
@@ -3357,7 +3350,7 @@
         <v>1.5</v>
       </c>
       <c r="I31" s="6">
-        <f>SUM(C31:H31)</f>
+        <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
       <c r="J31" s="4"/>
@@ -3410,7 +3403,7 @@
         <v>4</v>
       </c>
       <c r="I32" s="6">
-        <f>SUM(C32:H32)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="J32" s="4"/>
@@ -3463,7 +3456,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="6">
-        <f>SUM(C33:H33)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="J33" s="4"/>
@@ -3516,7 +3509,7 @@
         <v>2</v>
       </c>
       <c r="I34" s="6">
-        <f>SUM(C34:H34)</f>
+        <f t="shared" si="0"/>
         <v>14.5</v>
       </c>
       <c r="J34" s="4"/>
@@ -3569,7 +3562,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="6">
-        <f>SUM(C35:H35)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J35" s="4"/>
@@ -3622,7 +3615,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="6">
-        <f>SUM(C36:H36)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="J36" s="4"/>
@@ -3675,7 +3668,7 @@
         <v>2</v>
       </c>
       <c r="I37" s="6">
-        <f>SUM(C37:H37)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="J37" s="4"/>
@@ -3728,7 +3721,7 @@
         <v>4</v>
       </c>
       <c r="I38" s="6">
-        <f>SUM(C38:H38)</f>
+        <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
       <c r="J38" s="4"/>
@@ -3781,7 +3774,7 @@
         <v>1</v>
       </c>
       <c r="I39" s="6">
-        <f>SUM(C39:H39)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="J39" s="4"/>
@@ -3834,7 +3827,7 @@
         <v>2.5</v>
       </c>
       <c r="I40" s="6">
-        <f>SUM(C40:H40)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="J40" s="4"/>
@@ -3887,7 +3880,7 @@
         <v>2</v>
       </c>
       <c r="I41" s="6">
-        <f>SUM(C41:H41)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="J41" s="4"/>
@@ -3940,7 +3933,7 @@
         <v>2.5</v>
       </c>
       <c r="I42" s="6">
-        <f>SUM(C42:H42)</f>
+        <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
       <c r="J42" s="4"/>
@@ -3993,7 +3986,7 @@
         <v>2</v>
       </c>
       <c r="I43" s="6">
-        <f>SUM(C43:H43)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J43" s="4"/>
@@ -4046,7 +4039,7 @@
         <v>2</v>
       </c>
       <c r="I44" s="6">
-        <f>SUM(C44:H44)</f>
+        <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
       <c r="J44" s="4"/>
@@ -4099,7 +4092,7 @@
         <v>2</v>
       </c>
       <c r="I45" s="6">
-        <f>SUM(C45:H45)</f>
+        <f t="shared" si="0"/>
         <v>21.5</v>
       </c>
       <c r="J45" s="4"/>
@@ -4152,7 +4145,7 @@
         <v>2</v>
       </c>
       <c r="I46" s="6">
-        <f>SUM(C46:H46)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="J46" s="4"/>
@@ -4205,7 +4198,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="6">
-        <f>SUM(C47:H47)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="J47" s="4"/>
@@ -4258,7 +4251,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="6">
-        <f>SUM(C48:H48)</f>
+        <f t="shared" si="0"/>
         <v>19.5</v>
       </c>
       <c r="J48" s="4"/>
@@ -4293,17 +4286,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="AF1:AF3"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="B1:B4"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="AF1:AF3"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="AA1:AA2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I5:I48">
@@ -4317,10 +4310,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65546539-EC6B-4891-A0C5-BC2495986540}">
-  <dimension ref="A1:AF61"/>
+  <dimension ref="A1:AF62"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4344,10 +4337,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="40" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="32" t="s">
@@ -4358,7 +4351,7 @@
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
       <c r="H1" s="32"/>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="33" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="32" t="s">
@@ -4371,7 +4364,7 @@
       </c>
       <c r="N1" s="32"/>
       <c r="O1" s="32"/>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="33" t="s">
         <v>9</v>
       </c>
       <c r="Q1" s="32" t="s">
@@ -4386,22 +4379,22 @@
       <c r="X1" s="12"/>
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
-      <c r="AA1" s="41" t="s">
+      <c r="AA1" s="33" t="s">
         <v>9</v>
       </c>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="38" t="s">
+      <c r="AE1" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="42" t="s">
+      <c r="AF1" s="34" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -4420,7 +4413,7 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="41"/>
+      <c r="I2" s="33"/>
       <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
@@ -4439,7 +4432,7 @@
       <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="41"/>
+      <c r="P2" s="33"/>
       <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
@@ -4464,7 +4457,7 @@
       <c r="X2" s="12"/>
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
-      <c r="AA2" s="41"/>
+      <c r="AA2" s="33"/>
       <c r="AB2" s="1" t="s">
         <v>3</v>
       </c>
@@ -4474,12 +4467,12 @@
       <c r="AD2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AE2" s="39"/>
-      <c r="AF2" s="42"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="34"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
@@ -4548,12 +4541,12 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
-      <c r="AE3" s="40"/>
-      <c r="AF3" s="42"/>
+      <c r="AE3" s="42"/>
+      <c r="AF3" s="34"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="1">
         <v>6</v>
       </c>
@@ -7364,19 +7357,25 @@
         <v>18.5</v>
       </c>
     </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I62" s="45">
+        <f>AVERAGE(I5:I61)</f>
+        <v>12.315789473684211</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AF1:AF3"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="AE1:AE3"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="J1:L1"/>
+    <mergeCell ref="AF1:AF3"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="AE1:AE3"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="AA1:AA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7387,8 +7386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA98290-49A0-49FA-AB92-6C7AB89CB798}">
   <dimension ref="A1:AF58"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7427,7 +7426,7 @@
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
       <c r="H1" s="32"/>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="33" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="32" t="s">
@@ -7440,7 +7439,7 @@
       </c>
       <c r="N1" s="32"/>
       <c r="O1" s="32"/>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="33" t="s">
         <v>9</v>
       </c>
       <c r="Q1" s="32" t="s">
@@ -7455,7 +7454,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="41" t="s">
+      <c r="AA1" s="33" t="s">
         <v>9</v>
       </c>
       <c r="AB1" s="1"/>
@@ -7464,7 +7463,7 @@
       <c r="AE1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="42" t="s">
+      <c r="AF1" s="34" t="s">
         <v>28</v>
       </c>
     </row>
@@ -7489,7 +7488,7 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="41"/>
+      <c r="I2" s="33"/>
       <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
@@ -7508,7 +7507,7 @@
       <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="41"/>
+      <c r="P2" s="33"/>
       <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
@@ -7533,7 +7532,7 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="41"/>
+      <c r="AA2" s="33"/>
       <c r="AB2" s="1" t="s">
         <v>3</v>
       </c>
@@ -7544,7 +7543,7 @@
         <v>5</v>
       </c>
       <c r="AE2" s="32"/>
-      <c r="AF2" s="42"/>
+      <c r="AF2" s="34"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="43"/>
@@ -7620,7 +7619,7 @@
       <c r="AE3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AF3" s="42"/>
+      <c r="AF3" s="34"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="43"/>
@@ -10428,7 +10427,10 @@
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
-      <c r="I56" s="6"/>
+      <c r="I56" s="6">
+        <f>AVERAGE(I5:I55)</f>
+        <v>13.362745098039216</v>
+      </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
@@ -10479,17 +10481,17 @@
     </sortState>
   </autoFilter>
   <mergeCells count="11">
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AF1:AF3"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:L1"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AF1:AF3"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="AA1:AA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>